<commit_message>
Updated loot in the Solar Temple dungeon
</commit_message>
<xml_diff>
--- a/Solar Temple.xlsx
+++ b/Solar Temple.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>R</t>
   </si>
@@ -85,6 +85,54 @@
   </si>
   <si>
     <t>Once they kill the elemental the core/heart will be dropped</t>
+  </si>
+  <si>
+    <t>Once they win the fight, or if they flee the fight, they may decide to search the temple</t>
+  </si>
+  <si>
+    <t>If they do they will continue to find it mysteriously undisturbed, with  a stone cold but still "fresh" pot of soup on the stove in the kitchen.</t>
+  </si>
+  <si>
+    <t>If they fully leave the Central chamber when they return to it all signs of the fight will be gone, including bodies and potential loot</t>
+  </si>
+  <si>
+    <t>In the rest of the Temple they will find nothing of note, most of the chests in the bedrooms/barracks have been hacked apart, either by cultists or other opportunists</t>
+  </si>
+  <si>
+    <t>In the Janitors closet they will find a pair of old gloves and a ring</t>
+  </si>
+  <si>
+    <t>Gloves are gloves of climbing, ring is ring of slowfall.</t>
+  </si>
+  <si>
+    <t>There is a hidden room behind one of the bedroom, can be detected by spells, or a DC 18 investifation check</t>
+  </si>
+  <si>
+    <t>To access the room they will have to break through the wall (Very hard) or solve a riddle (Found in the priests diary in the room)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the room they will find </t>
+  </si>
+  <si>
+    <t>Cask of expensive wiskey (200 gold)</t>
+  </si>
+  <si>
+    <t>Magical Elemental Figurine (When smashed releases a bound solar elemental)</t>
+  </si>
+  <si>
+    <t>Scroll of Magic Circle</t>
+  </si>
+  <si>
+    <t>The room appears to have been used to hide things that where to heavy/magically potent to hide when the priests fled the temple.</t>
+  </si>
+  <si>
+    <t>A small chest of gold bars (400 gold)</t>
+  </si>
+  <si>
+    <t>Silver Candle Sticks (100 Gold)</t>
+  </si>
+  <si>
+    <t>Spell Book with 3 random lvl 1 spells and 1 lvl 2 spell</t>
   </si>
 </sst>
 </file>
@@ -462,71 +510,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -603,6 +597,60 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F4:BV28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AL23" sqref="AL23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,24 +947,24 @@
     </row>
     <row r="7" spans="6:73" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="6:73" x14ac:dyDescent="0.25">
-      <c r="M8" s="77"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="79"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="61"/>
       <c r="U8" s="1"/>
       <c r="V8" s="2"/>
-      <c r="AB8" s="98"/>
-      <c r="AC8" s="99"/>
-      <c r="AD8" s="100"/>
+      <c r="AB8" s="80"/>
+      <c r="AC8" s="81"/>
+      <c r="AD8" s="82"/>
     </row>
     <row r="9" spans="6:73" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M9" s="75"/>
-      <c r="N9" s="88"/>
-      <c r="O9" s="74"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="70"/>
+      <c r="O9" s="56"/>
       <c r="U9" s="3"/>
       <c r="V9" s="4"/>
-      <c r="AB9" s="101"/>
-      <c r="AC9" s="102"/>
-      <c r="AD9" s="103"/>
+      <c r="AB9" s="83"/>
+      <c r="AC9" s="84"/>
+      <c r="AD9" s="85"/>
       <c r="AH9" s="11"/>
     </row>
     <row r="10" spans="6:73" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -964,9 +1012,9 @@
       <c r="BU12" s="11"/>
     </row>
     <row r="13" spans="6:73" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I13" s="68"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="70"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="52"/>
       <c r="L13" s="2"/>
       <c r="R13" s="3"/>
       <c r="S13" s="11"/>
@@ -981,9 +1029,9 @@
       <c r="AC13" s="18"/>
       <c r="AE13" s="1"/>
       <c r="AF13" s="8"/>
-      <c r="AG13" s="89"/>
-      <c r="AH13" s="90"/>
-      <c r="AI13" s="91"/>
+      <c r="AG13" s="71"/>
+      <c r="AH13" s="72"/>
+      <c r="AI13" s="73"/>
       <c r="BL13" s="7"/>
       <c r="BM13" s="11"/>
       <c r="BO13" s="5"/>
@@ -996,12 +1044,12 @@
       </c>
     </row>
     <row r="14" spans="6:73" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F14" s="51"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="62"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="44"/>
       <c r="L14" s="12"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
@@ -1022,21 +1070,21 @@
       <c r="AA14" s="11"/>
       <c r="AD14" s="8"/>
       <c r="AE14" s="6"/>
-      <c r="AG14" s="92"/>
-      <c r="AH14" s="93"/>
-      <c r="AI14" s="94"/>
-      <c r="AJ14" s="77"/>
-      <c r="AK14" s="78"/>
-      <c r="AL14" s="79"/>
+      <c r="AG14" s="74"/>
+      <c r="AH14" s="75"/>
+      <c r="AI14" s="76"/>
+      <c r="AJ14" s="59"/>
+      <c r="AK14" s="60"/>
+      <c r="AL14" s="61"/>
       <c r="AS14" s="11"/>
     </row>
     <row r="15" spans="6:73" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F15" s="83"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="64"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="46"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="11"/>
       <c r="R15" s="11"/>
@@ -1051,24 +1099,24 @@
       <c r="AA15" s="4"/>
       <c r="AB15" s="17"/>
       <c r="AC15" s="17"/>
-      <c r="AG15" s="95"/>
-      <c r="AH15" s="96"/>
-      <c r="AI15" s="97"/>
-      <c r="AJ15" s="80"/>
-      <c r="AK15" s="81"/>
-      <c r="AL15" s="76"/>
-      <c r="AS15" s="46" t="s">
+      <c r="AG15" s="77"/>
+      <c r="AH15" s="78"/>
+      <c r="AI15" s="79"/>
+      <c r="AJ15" s="62"/>
+      <c r="AK15" s="63"/>
+      <c r="AL15" s="58"/>
+      <c r="AS15" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="AT15" s="46"/>
-      <c r="AU15" s="46"/>
-      <c r="AV15" s="46"/>
-      <c r="AY15" s="104" t="s">
+      <c r="AT15" s="28"/>
+      <c r="AU15" s="28"/>
+      <c r="AV15" s="28"/>
+      <c r="AY15" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="AZ15" s="104"/>
-      <c r="BA15" s="104"/>
-      <c r="BB15" s="104"/>
+      <c r="AZ15" s="86"/>
+      <c r="BA15" s="86"/>
+      <c r="BB15" s="86"/>
       <c r="BF15" s="11"/>
       <c r="BI15" s="11"/>
       <c r="BL15" s="11"/>
@@ -1076,7 +1124,7 @@
       <c r="BU15" s="11"/>
     </row>
     <row r="16" spans="6:73" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O16" s="22" t="s">
+      <c r="O16" s="94" t="s">
         <v>2</v>
       </c>
       <c r="P16" s="11"/>
@@ -1085,13 +1133,13 @@
       <c r="S16" s="11"/>
       <c r="T16" s="18"/>
       <c r="U16" s="1"/>
-      <c r="V16" s="31"/>
+      <c r="V16" s="21"/>
       <c r="W16" s="5"/>
       <c r="X16" s="11"/>
       <c r="Y16" s="11"/>
       <c r="Z16" s="11"/>
       <c r="AA16" s="11"/>
-      <c r="AB16" s="25" t="s">
+      <c r="AB16" s="97" t="s">
         <v>2</v>
       </c>
       <c r="BL16" s="14"/>
@@ -1102,28 +1150,28 @@
       <c r="BU16" s="4"/>
     </row>
     <row r="17" spans="9:74" x14ac:dyDescent="0.25">
-      <c r="O17" s="23"/>
+      <c r="O17" s="95"/>
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
       <c r="S17" s="4"/>
-      <c r="T17" s="33" t="s">
+      <c r="T17" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="U17" s="30"/>
-      <c r="V17" s="30"/>
-      <c r="W17" s="34"/>
+      <c r="U17" s="104"/>
+      <c r="V17" s="104"/>
+      <c r="W17" s="105"/>
       <c r="X17" s="3"/>
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
       <c r="AA17" s="11"/>
-      <c r="AB17" s="26"/>
-      <c r="AS17" s="59" t="s">
+      <c r="AB17" s="98"/>
+      <c r="AS17" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="AT17" s="59"/>
-      <c r="AU17" s="59"/>
-      <c r="AV17" s="59"/>
+      <c r="AT17" s="41"/>
+      <c r="AU17" s="41"/>
+      <c r="AV17" s="41"/>
       <c r="BC17" s="11"/>
       <c r="BD17" s="11"/>
       <c r="BE17" s="11"/>
@@ -1135,43 +1183,43 @@
       <c r="BU17" s="11"/>
     </row>
     <row r="18" spans="9:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O18" s="23"/>
+      <c r="O18" s="95"/>
       <c r="P18" s="11"/>
       <c r="Q18" s="11"/>
       <c r="R18" s="11"/>
       <c r="S18" s="4"/>
-      <c r="T18" s="33"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="30"/>
-      <c r="W18" s="34"/>
+      <c r="T18" s="103"/>
+      <c r="U18" s="104"/>
+      <c r="V18" s="104"/>
+      <c r="W18" s="105"/>
       <c r="X18" s="3"/>
       <c r="Y18" s="11"/>
       <c r="Z18" s="11"/>
       <c r="AA18" s="11"/>
-      <c r="AB18" s="26"/>
+      <c r="AB18" s="98"/>
       <c r="BR18" s="11"/>
     </row>
     <row r="19" spans="9:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O19" s="24"/>
+      <c r="O19" s="96"/>
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
       <c r="T19" s="2"/>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
       <c r="W19" s="1"/>
       <c r="X19" s="11"/>
       <c r="Y19" s="11"/>
       <c r="Z19" s="11"/>
       <c r="AA19" s="11"/>
-      <c r="AB19" s="27"/>
-      <c r="AS19" s="65" t="s">
+      <c r="AB19" s="99"/>
+      <c r="AS19" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="AT19" s="65"/>
-      <c r="AU19" s="65"/>
-      <c r="AV19" s="65"/>
+      <c r="AT19" s="47"/>
+      <c r="AU19" s="47"/>
+      <c r="AV19" s="47"/>
       <c r="BL19" s="9"/>
       <c r="BN19" s="11"/>
       <c r="BO19" s="2"/>
@@ -1185,9 +1233,9 @@
       <c r="BV19" s="11"/>
     </row>
     <row r="20" spans="9:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K20" s="51"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="53"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="35"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
@@ -1202,18 +1250,18 @@
       <c r="AA20" s="4"/>
       <c r="AB20" s="18"/>
       <c r="AC20" s="18"/>
-      <c r="AD20" s="51"/>
-      <c r="AE20" s="56"/>
-      <c r="AF20" s="53"/>
+      <c r="AD20" s="33"/>
+      <c r="AE20" s="38"/>
+      <c r="AF20" s="35"/>
       <c r="AG20" s="18"/>
       <c r="BU20" s="11"/>
     </row>
     <row r="21" spans="9:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="35"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
       <c r="N21" s="16"/>
       <c r="O21" s="8"/>
       <c r="P21" s="12"/>
@@ -1230,20 +1278,20 @@
       <c r="AA21" s="18"/>
       <c r="AB21" s="18"/>
       <c r="AC21" s="18"/>
-      <c r="AD21" s="58"/>
-      <c r="AE21" s="57"/>
-      <c r="AF21" s="57"/>
-      <c r="AG21" s="50"/>
-      <c r="AH21" s="49"/>
-      <c r="AS21" s="82" t="s">
+      <c r="AD21" s="40"/>
+      <c r="AE21" s="39"/>
+      <c r="AF21" s="39"/>
+      <c r="AG21" s="32"/>
+      <c r="AH21" s="31"/>
+      <c r="AS21" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="AT21" s="82"/>
-      <c r="AU21" s="82"/>
-      <c r="AV21" s="82"/>
+      <c r="AT21" s="64"/>
+      <c r="AU21" s="64"/>
+      <c r="AV21" s="64"/>
     </row>
     <row r="22" spans="9:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I22" s="37"/>
+      <c r="I22" s="25"/>
       <c r="R22" s="3"/>
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
@@ -1255,15 +1303,15 @@
       <c r="Z22" s="18"/>
       <c r="AA22" s="18"/>
       <c r="AG22" s="9"/>
-      <c r="AH22" s="46"/>
+      <c r="AH22" s="28"/>
       <c r="AI22" s="3"/>
     </row>
     <row r="23" spans="9:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I23" s="38"/>
-      <c r="J23" s="40" t="s">
+      <c r="I23" s="26"/>
+      <c r="J23" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="K23" s="41"/>
+      <c r="K23" s="89"/>
       <c r="O23" s="19"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="8"/>
@@ -1277,110 +1325,110 @@
       <c r="Y23" s="18"/>
       <c r="Z23" s="8"/>
       <c r="AA23" s="18"/>
-      <c r="AB23" s="32"/>
+      <c r="AB23" s="22"/>
       <c r="AC23" s="3"/>
-      <c r="AF23" s="35" t="s">
+      <c r="AF23" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AG23" s="46"/>
-      <c r="AH23" s="46"/>
+      <c r="AG23" s="28"/>
+      <c r="AH23" s="28"/>
       <c r="AI23" s="3"/>
-      <c r="AS23" s="85" t="s">
+      <c r="AS23" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="AT23" s="85"/>
-      <c r="AU23" s="85"/>
-      <c r="AV23" s="85"/>
+      <c r="AT23" s="67"/>
+      <c r="AU23" s="67"/>
+      <c r="AV23" s="67"/>
     </row>
     <row r="24" spans="9:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="38"/>
-      <c r="J24" s="42" t="s">
+      <c r="I24" s="26"/>
+      <c r="J24" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="K24" s="43"/>
-      <c r="O24" s="60"/>
-      <c r="P24" s="61"/>
-      <c r="T24" s="28" t="s">
+      <c r="K24" s="91"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="43"/>
+      <c r="T24" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="U24" s="29"/>
-      <c r="V24" s="29"/>
-      <c r="W24" s="21"/>
-      <c r="AA24" s="60"/>
-      <c r="AB24" s="65"/>
+      <c r="U24" s="101"/>
+      <c r="V24" s="101"/>
+      <c r="W24" s="102"/>
+      <c r="AA24" s="42"/>
+      <c r="AB24" s="47"/>
       <c r="AC24" s="3"/>
-      <c r="AF24" s="38" t="s">
+      <c r="AF24" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="AG24" s="46"/>
-      <c r="AH24" s="46"/>
+      <c r="AG24" s="28"/>
+      <c r="AH24" s="28"/>
       <c r="AI24" s="3"/>
     </row>
     <row r="25" spans="9:74" x14ac:dyDescent="0.25">
-      <c r="I25" s="38"/>
-      <c r="J25" s="42" t="s">
+      <c r="I25" s="26"/>
+      <c r="J25" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="K25" s="43"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="62"/>
-      <c r="AA25" s="60"/>
-      <c r="AB25" s="65"/>
+      <c r="K25" s="91"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="44"/>
+      <c r="AA25" s="42"/>
+      <c r="AB25" s="47"/>
       <c r="AC25" s="3"/>
-      <c r="AF25" s="38" t="s">
+      <c r="AF25" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="AG25" s="46"/>
-      <c r="AH25" s="46"/>
+      <c r="AG25" s="28"/>
+      <c r="AH25" s="28"/>
       <c r="AI25" s="3"/>
-      <c r="AS25" s="93" t="s">
+      <c r="AS25" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="AT25" s="93"/>
-      <c r="AU25" s="93"/>
-      <c r="AV25" s="93"/>
+      <c r="AT25" s="75"/>
+      <c r="AU25" s="75"/>
+      <c r="AV25" s="75"/>
     </row>
     <row r="26" spans="9:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I26" s="39"/>
-      <c r="J26" s="44" t="s">
+      <c r="I26" s="27"/>
+      <c r="J26" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="K26" s="45"/>
-      <c r="O26" s="63"/>
-      <c r="P26" s="64"/>
-      <c r="AA26" s="66"/>
-      <c r="AB26" s="67"/>
+      <c r="K26" s="93"/>
+      <c r="O26" s="45"/>
+      <c r="P26" s="46"/>
+      <c r="AA26" s="48"/>
+      <c r="AB26" s="49"/>
       <c r="AC26" s="3"/>
-      <c r="AF26" s="39" t="s">
+      <c r="AF26" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="AG26" s="47"/>
-      <c r="AH26" s="48"/>
+      <c r="AG26" s="29"/>
+      <c r="AH26" s="30"/>
     </row>
     <row r="27" spans="9:74" x14ac:dyDescent="0.25">
-      <c r="O27" s="73"/>
-      <c r="P27" s="74"/>
-      <c r="AA27" s="84"/>
-      <c r="AB27" s="85"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="56"/>
+      <c r="AA27" s="66"/>
+      <c r="AB27" s="67"/>
       <c r="AC27" s="3"/>
     </row>
     <row r="28" spans="9:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O28" s="75"/>
-      <c r="P28" s="76"/>
-      <c r="AA28" s="86"/>
-      <c r="AB28" s="87"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="58"/>
+      <c r="AA28" s="68"/>
+      <c r="AB28" s="69"/>
       <c r="AC28" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="AB16:AB19"/>
+    <mergeCell ref="T24:W24"/>
+    <mergeCell ref="T17:W18"/>
     <mergeCell ref="J23:K23"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="J25:K25"/>
     <mergeCell ref="J26:K26"/>
     <mergeCell ref="O16:O19"/>
-    <mergeCell ref="AB16:AB19"/>
-    <mergeCell ref="T24:W24"/>
-    <mergeCell ref="T17:W18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1389,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D11"/>
+  <dimension ref="B2:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,6 +1490,86 @@
         <v>19</v>
       </c>
     </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>